<commit_message>
Feature #3323: old livestock wagon (graphics by Voyager One) (closes #3323)
</commit_message>
<xml_diff>
--- a/docs/cargo_classes.xlsx
+++ b/docs/cargo_classes.xlsx
@@ -11,14 +11,14 @@
     <sheet name="Wagons" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Cargo!$A$1:$AE$68</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Cargo!$A$1:$AG$68</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="425" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="171">
   <si>
     <t>Label</t>
   </si>
@@ -525,6 +525,12 @@
   </si>
   <si>
     <t>In CTT</t>
+  </si>
+  <si>
+    <t>Livestock wagon</t>
+  </si>
+  <si>
+    <t>only</t>
   </si>
 </sst>
 </file>
@@ -566,7 +572,27 @@
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -874,14 +900,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:AF68"/>
+  <dimension ref="A1:AG68"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="K2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G65" sqref="G65"/>
+      <selection pane="bottomRight" activeCell="AG7" sqref="AG7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -893,7 +918,7 @@
     <col min="19" max="29" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -990,8 +1015,11 @@
       <c r="AF1" t="s">
         <v>167</v>
       </c>
-    </row>
-    <row r="2" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
+      <c r="AG1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1018,7 +1046,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1048,7 +1076,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1075,7 +1103,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1102,7 +1130,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -1128,8 +1156,11 @@
       <c r="U6">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -1159,7 +1190,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -1192,7 +1223,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -1219,7 +1250,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -1249,7 +1280,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -1279,7 +1310,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -1303,7 +1334,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -1333,7 +1364,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>29</v>
       </c>
@@ -1363,7 +1394,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -1399,7 +1430,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -1423,7 +1454,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:31" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -1456,7 +1487,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:31" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>37</v>
       </c>
@@ -1492,7 +1523,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:31" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>39</v>
       </c>
@@ -1522,7 +1553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:31" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>41</v>
       </c>
@@ -1549,7 +1580,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:31" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>43</v>
       </c>
@@ -1576,7 +1607,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:31" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>45</v>
       </c>
@@ -1600,7 +1631,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:31" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>47</v>
       </c>
@@ -1636,7 +1667,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:31" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>49</v>
       </c>
@@ -1657,7 +1688,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:31" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>51</v>
       </c>
@@ -1699,7 +1730,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:31" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>55</v>
       </c>
@@ -1720,7 +1751,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:31" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>57</v>
       </c>
@@ -1744,7 +1775,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:31" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>59</v>
       </c>
@@ -1765,7 +1796,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:31" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>61</v>
       </c>
@@ -1786,7 +1817,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:31" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>63</v>
       </c>
@@ -1813,7 +1844,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:31" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>65</v>
       </c>
@@ -1837,7 +1868,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:31" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>67</v>
       </c>
@@ -1903,7 +1934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:31" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>71</v>
       </c>
@@ -1939,7 +1970,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:31" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>73</v>
       </c>
@@ -1966,7 +1997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:31" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>75</v>
       </c>
@@ -1993,7 +2024,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:31" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>77</v>
       </c>
@@ -2029,7 +2060,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:31" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>79</v>
       </c>
@@ -2059,7 +2090,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:31" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>81</v>
       </c>
@@ -2098,7 +2129,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:31" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>83</v>
       </c>
@@ -2122,7 +2153,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:31" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>85</v>
       </c>
@@ -2188,7 +2219,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:31" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>89</v>
       </c>
@@ -2227,7 +2258,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:31" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>91</v>
       </c>
@@ -2371,7 +2402,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>99</v>
       </c>
@@ -2401,7 +2432,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>101</v>
       </c>
@@ -2428,7 +2459,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>103</v>
       </c>
@@ -2524,7 +2555,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>109</v>
       </c>
@@ -2560,7 +2591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>111</v>
       </c>
@@ -2587,7 +2618,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>63</v>
       </c>
@@ -2620,7 +2651,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>114</v>
       </c>
@@ -2653,7 +2684,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>116</v>
       </c>
@@ -2692,7 +2723,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>118</v>
       </c>
@@ -2719,7 +2750,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>120</v>
       </c>
@@ -2749,7 +2780,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>122</v>
       </c>
@@ -2776,7 +2807,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>124</v>
       </c>
@@ -2803,7 +2834,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>126</v>
       </c>
@@ -2830,7 +2861,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:32" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>128</v>
       </c>
@@ -2890,7 +2921,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>132</v>
       </c>
@@ -2917,7 +2948,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>134</v>
       </c>
@@ -2956,7 +2987,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:28" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>136</v>
       </c>
@@ -2990,23 +3021,17 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AE68">
-    <filterColumn colId="6">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:AG68"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AL15"/>
+  <dimension ref="A1:AL16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3824,6 +3849,9 @@
         <f>SUMIF(Cargo!$AC:$AC,1,Cargo!O:O)</f>
         <v>0</v>
       </c>
+      <c r="P12" t="s">
+        <v>170</v>
+      </c>
       <c r="Q12" t="s">
         <v>16</v>
       </c>
@@ -3891,6 +3919,9 @@
         <f>SUMIF(Cargo!$AD:$AD,1,Cargo!O:O)</f>
         <v>0</v>
       </c>
+      <c r="P13" t="s">
+        <v>170</v>
+      </c>
       <c r="Q13" t="s">
         <v>22</v>
       </c>
@@ -3946,6 +3977,9 @@
         <f>SUMIF(Cargo!$AE:$AE,1,Cargo!O:O)</f>
         <v>0</v>
       </c>
+      <c r="P14" t="s">
+        <v>170</v>
+      </c>
       <c r="Q14" t="s">
         <v>46</v>
       </c>
@@ -4013,13 +4047,71 @@
         <f>SUMIF(Cargo!$AF:$AF,1,Cargo!O:O)</f>
         <v>0</v>
       </c>
+      <c r="P15" t="s">
+        <v>170</v>
+      </c>
       <c r="Q15" t="s">
         <v>115</v>
       </c>
     </row>
+    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>169</v>
+      </c>
+      <c r="B16">
+        <f>SUMIF(Cargo!$AG:$AG,1,Cargo!E:E)</f>
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <f>SUMIF(Cargo!$AG:$AG,1,Cargo!F:F)</f>
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <f>SUMIF(Cargo!$AG:$AG,1,Cargo!G:G)</f>
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <f>SUMIF(Cargo!$AG:$AG,1,Cargo!H:H)</f>
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <f>SUMIF(Cargo!$AG:$AG,1,Cargo!I:I)</f>
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <f>SUMIF(Cargo!$AG:$AG,1,Cargo!J:J)</f>
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <f>SUMIF(Cargo!$AG:$AG,1,Cargo!K:K)</f>
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <f>SUMIF(Cargo!$AG:$AG,1,Cargo!L:L)</f>
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <f>SUMIF(Cargo!$AG:$AG,1,Cargo!M:M)</f>
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <f>SUMIF(Cargo!$AG:$AG,1,Cargo!N:N)</f>
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <f>SUMIF(Cargo!$AG:$AG,1,Cargo!O:O)</f>
+        <v>0</v>
+      </c>
+      <c r="P16" t="s">
+        <v>170</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:L15">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+  <conditionalFormatting sqref="B2:L16">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Change: allow mail and armoured cargo in first boxcar (issue #4136)
</commit_message>
<xml_diff>
--- a/docs/cargo_classes.xlsx
+++ b/docs/cargo_classes.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="135" windowWidth="21075" windowHeight="9525"/>
@@ -10,14 +10,14 @@
     <sheet name="Cargo" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Cargo!$A$1:$AT$82</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Cargo!$A$1:$AU$82</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="182">
   <si>
     <t>Label</t>
   </si>
@@ -560,6 +560,9 @@
   </si>
   <si>
     <t>Flat wagon w/o stakes</t>
+  </si>
+  <si>
+    <t>Boxcar w Mail+Armoured</t>
   </si>
 </sst>
 </file>
@@ -923,13 +926,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AT82"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:AU82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2:B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -948,10 +952,12 @@
     <col min="28" max="29" width="3.7109375" customWidth="1"/>
     <col min="30" max="30" width="3.7109375" bestFit="1" customWidth="1"/>
     <col min="31" max="35" width="3.7109375" customWidth="1"/>
-    <col min="36" max="46" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="36" max="37" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="3.7109375" customWidth="1"/>
+    <col min="39" max="47" width="3.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" s="1" customFormat="1" ht="123.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:47" s="1" customFormat="1" ht="123.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1064,34 +1070,37 @@
         <v>167</v>
       </c>
       <c r="AL1" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="AM1" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="AT1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="2" spans="1:46" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -1128,12 +1137,12 @@
         <f>IF(OR(AG2=1,AH2=1),1,"")</f>
         <v/>
       </c>
-      <c r="AM2" s="3" t="str">
-        <f>IF(OR(AN2=1,AL2=1),1,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="3" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AN2" s="3" t="str">
+        <f>IF(OR(AO2=1,AM2=1),1,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1166,12 +1175,12 @@
       <c r="AD3">
         <v>1</v>
       </c>
-      <c r="AM3" s="3" t="str">
-        <f t="shared" ref="AM3:AM66" si="2">IF(OR(AN3=1,AL3=1),1,"")</f>
-        <v/>
-      </c>
-    </row>
-    <row r="4" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AN3" s="3" t="str">
+        <f t="shared" ref="AN3:AN66" si="2">IF(OR(AO3=1,AM3=1),1,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1214,12 +1223,15 @@
         <f t="shared" ref="AF4:AF7" si="3">IF(OR(AG4=1,AH4=1),1,"")</f>
         <v/>
       </c>
-      <c r="AM4" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="5" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AL4">
+        <v>1</v>
+      </c>
+      <c r="AN4" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -1250,15 +1262,15 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="AM5" s="3">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="AN5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AN5" s="3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AO5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -1289,15 +1301,15 @@
         <f t="shared" si="3"/>
         <v/>
       </c>
-      <c r="AM6" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="AQ6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AN6" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AR6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -1343,12 +1355,15 @@
       <c r="AL7">
         <v>1</v>
       </c>
-      <c r="AM7" s="3">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AM7">
+        <v>1</v>
+      </c>
+      <c r="AN7" s="3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -1381,15 +1396,18 @@
       <c r="AK8">
         <v>1</v>
       </c>
-      <c r="AM8" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="AO8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AL8">
+        <v>1</v>
+      </c>
+      <c r="AN8" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AP8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -1423,12 +1441,12 @@
       <c r="AH9">
         <v>1</v>
       </c>
-      <c r="AM9" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="10" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AN9" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -1461,12 +1479,12 @@
       <c r="AD10">
         <v>1</v>
       </c>
-      <c r="AM10" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="11" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AN10" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -1500,15 +1518,15 @@
       <c r="AH11">
         <v>1</v>
       </c>
-      <c r="AM11" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="AP11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AN11" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AQ11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -1542,12 +1560,15 @@
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="AM12" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="13" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AL12">
+        <v>1</v>
+      </c>
+      <c r="AN12" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -1584,12 +1605,15 @@
       <c r="AL13">
         <v>1</v>
       </c>
-      <c r="AM13" s="3">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AM13">
+        <v>1</v>
+      </c>
+      <c r="AN13" s="3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>29</v>
       </c>
@@ -1619,15 +1643,18 @@
       <c r="AK14">
         <v>1</v>
       </c>
-      <c r="AM14" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="AO14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AL14">
+        <v>1</v>
+      </c>
+      <c r="AN14" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AP14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -1676,12 +1703,15 @@
       <c r="AL15">
         <v>1</v>
       </c>
-      <c r="AM15" s="3">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AM15">
+        <v>1</v>
+      </c>
+      <c r="AN15" s="3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -1715,12 +1745,15 @@
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="AM16" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="17" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AL16">
+        <v>1</v>
+      </c>
+      <c r="AN16" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="17" spans="1:46" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -1753,15 +1786,18 @@
       <c r="AL17">
         <v>1</v>
       </c>
-      <c r="AM17" s="3">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="AN17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AM17">
+        <v>1</v>
+      </c>
+      <c r="AN17" s="3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AO17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:46" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>37</v>
       </c>
@@ -1800,12 +1836,15 @@
       <c r="AL18">
         <v>1</v>
       </c>
-      <c r="AM18" s="3">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AM18">
+        <v>1</v>
+      </c>
+      <c r="AN18" s="3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:46" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>39</v>
       </c>
@@ -1835,15 +1874,18 @@
       <c r="AK19">
         <v>1</v>
       </c>
-      <c r="AM19" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="AO19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AL19">
+        <v>1</v>
+      </c>
+      <c r="AN19" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AP19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>41</v>
       </c>
@@ -1873,12 +1915,12 @@
       <c r="AD20">
         <v>1</v>
       </c>
-      <c r="AM20" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="21" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AN20" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:46" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>43</v>
       </c>
@@ -1912,15 +1954,18 @@
       <c r="AL21">
         <v>1</v>
       </c>
-      <c r="AM21" s="3">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="AN21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AM21">
+        <v>1</v>
+      </c>
+      <c r="AN21" s="3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AO21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:46" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>45</v>
       </c>
@@ -1954,12 +1999,15 @@
         <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="AM22" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="23" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AL22">
+        <v>1</v>
+      </c>
+      <c r="AN22" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="1:46" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>47</v>
       </c>
@@ -1992,18 +2040,21 @@
       <c r="AL23">
         <v>1</v>
       </c>
-      <c r="AM23" s="3">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="AO23">
-        <v>1</v>
-      </c>
-      <c r="AS23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AM23">
+        <v>1</v>
+      </c>
+      <c r="AN23" s="3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AP23">
+        <v>1</v>
+      </c>
+      <c r="AT23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:46" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>49</v>
       </c>
@@ -2034,12 +2085,15 @@
       <c r="AL24">
         <v>1</v>
       </c>
-      <c r="AM24" s="3">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AM24">
+        <v>1</v>
+      </c>
+      <c r="AN24" s="3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:46" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>51</v>
       </c>
@@ -2070,12 +2124,15 @@
       <c r="AL25">
         <v>1</v>
       </c>
-      <c r="AM25" s="3">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AM25">
+        <v>1</v>
+      </c>
+      <c r="AN25" s="3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:46" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>53</v>
       </c>
@@ -2106,12 +2163,15 @@
       <c r="AL26">
         <v>1</v>
       </c>
-      <c r="AM26" s="3">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AM26">
+        <v>1</v>
+      </c>
+      <c r="AN26" s="3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:46" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>55</v>
       </c>
@@ -2142,12 +2202,15 @@
       <c r="AL27">
         <v>1</v>
       </c>
-      <c r="AM27" s="3">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AM27">
+        <v>1</v>
+      </c>
+      <c r="AN27" s="3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:46" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>57</v>
       </c>
@@ -2178,15 +2241,18 @@
       <c r="AL28">
         <v>1</v>
       </c>
-      <c r="AM28" s="3">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="AN28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AM28">
+        <v>1</v>
+      </c>
+      <c r="AN28" s="3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AO28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:46" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>59</v>
       </c>
@@ -2217,12 +2283,15 @@
       <c r="AL29">
         <v>1</v>
       </c>
-      <c r="AM29" s="3">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AM29">
+        <v>1</v>
+      </c>
+      <c r="AN29" s="3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:46" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>61</v>
       </c>
@@ -2253,12 +2322,15 @@
       <c r="AL30">
         <v>1</v>
       </c>
-      <c r="AM30" s="3">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AM30">
+        <v>1</v>
+      </c>
+      <c r="AN30" s="3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:46" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>63</v>
       </c>
@@ -2292,18 +2364,21 @@
       <c r="AL31">
         <v>1</v>
       </c>
-      <c r="AM31" s="3">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="AN31">
+      <c r="AM31">
+        <v>1</v>
+      </c>
+      <c r="AN31" s="3">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AO31">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AP31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:46" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>65</v>
       </c>
@@ -2334,15 +2409,18 @@
       <c r="AL32">
         <v>1</v>
       </c>
-      <c r="AM32" s="3">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="AN32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AM32">
+        <v>1</v>
+      </c>
+      <c r="AN32" s="3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AO32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>67</v>
       </c>
@@ -2375,12 +2453,12 @@
       <c r="AD33">
         <v>1</v>
       </c>
-      <c r="AM33" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="34" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AN33" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>69</v>
       </c>
@@ -2426,15 +2504,18 @@
       <c r="AL34">
         <v>1</v>
       </c>
-      <c r="AM34" s="3">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="AN34">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="35" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AM34">
+        <v>1</v>
+      </c>
+      <c r="AN34" s="3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AO34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>71</v>
       </c>
@@ -2477,18 +2558,21 @@
       <c r="AL35">
         <v>1</v>
       </c>
-      <c r="AM35" s="3">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="AO35">
-        <v>1</v>
-      </c>
-      <c r="AS35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AM35">
+        <v>1</v>
+      </c>
+      <c r="AN35" s="3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AP35">
+        <v>1</v>
+      </c>
+      <c r="AT35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>73</v>
       </c>
@@ -2521,12 +2605,15 @@
       <c r="AK36">
         <v>1</v>
       </c>
-      <c r="AM36" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="37" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AL36">
+        <v>1</v>
+      </c>
+      <c r="AN36" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="37" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>75</v>
       </c>
@@ -2560,12 +2647,15 @@
       <c r="AL37">
         <v>1</v>
       </c>
-      <c r="AM37" s="3">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AM37">
+        <v>1</v>
+      </c>
+      <c r="AN37" s="3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>77</v>
       </c>
@@ -2601,15 +2691,18 @@
       <c r="AK38">
         <v>1</v>
       </c>
-      <c r="AM38" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="AO38">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="39" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AL38">
+        <v>1</v>
+      </c>
+      <c r="AN38" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AP38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>79</v>
       </c>
@@ -2640,12 +2733,12 @@
       <c r="AD39">
         <v>1</v>
       </c>
-      <c r="AM39" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="40" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AN39" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="40" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>81</v>
       </c>
@@ -2684,18 +2777,21 @@
       <c r="AL40">
         <v>1</v>
       </c>
-      <c r="AM40" s="3">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="AO40">
-        <v>1</v>
-      </c>
-      <c r="AS40">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AM40">
+        <v>1</v>
+      </c>
+      <c r="AN40" s="3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AP40">
+        <v>1</v>
+      </c>
+      <c r="AT40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>83</v>
       </c>
@@ -2726,15 +2822,18 @@
       <c r="AK41">
         <v>1</v>
       </c>
-      <c r="AM41" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="AP41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AL41">
+        <v>1</v>
+      </c>
+      <c r="AN41" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AQ41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>85</v>
       </c>
@@ -2771,15 +2870,18 @@
       <c r="AL42">
         <v>1</v>
       </c>
-      <c r="AM42" s="3">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="AN42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AM42">
+        <v>1</v>
+      </c>
+      <c r="AN42" s="3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AO42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>87</v>
       </c>
@@ -2822,12 +2924,15 @@
       <c r="AL43">
         <v>1</v>
       </c>
-      <c r="AM43" s="3">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AM43">
+        <v>1</v>
+      </c>
+      <c r="AN43" s="3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>89</v>
       </c>
@@ -2866,18 +2971,21 @@
       <c r="AL44">
         <v>1</v>
       </c>
-      <c r="AM44" s="3">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="AS44">
+      <c r="AM44">
+        <v>1</v>
+      </c>
+      <c r="AN44" s="3">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AT44">
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AU44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>91</v>
       </c>
@@ -2916,12 +3024,15 @@
       <c r="AK45">
         <v>1</v>
       </c>
-      <c r="AM45" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="46" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AL45">
+        <v>1</v>
+      </c>
+      <c r="AN45" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="46" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>93</v>
       </c>
@@ -2964,15 +3075,18 @@
       <c r="AL46">
         <v>1</v>
       </c>
-      <c r="AM46" s="3">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="AN46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AM46">
+        <v>1</v>
+      </c>
+      <c r="AN46" s="3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AO46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>95</v>
       </c>
@@ -3015,15 +3129,18 @@
       <c r="AL47">
         <v>1</v>
       </c>
-      <c r="AM47" s="3">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="AT47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AM47">
+        <v>1</v>
+      </c>
+      <c r="AN47" s="3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AU47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>97</v>
       </c>
@@ -3066,12 +3183,15 @@
       <c r="AL48">
         <v>1</v>
       </c>
-      <c r="AM48" s="3">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AM48">
+        <v>1</v>
+      </c>
+      <c r="AN48" s="3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>99</v>
       </c>
@@ -3111,12 +3231,15 @@
       <c r="AL49">
         <v>1</v>
       </c>
-      <c r="AM49" s="3">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AM49">
+        <v>1</v>
+      </c>
+      <c r="AN49" s="3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>101</v>
       </c>
@@ -3146,12 +3269,12 @@
       <c r="AD50">
         <v>1</v>
       </c>
-      <c r="AM50" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="51" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AN50" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="51" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>103</v>
       </c>
@@ -3181,15 +3304,15 @@
       <c r="AD51">
         <v>1</v>
       </c>
-      <c r="AM51" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="AS51">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AN51" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AT51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>105</v>
       </c>
@@ -3232,15 +3355,18 @@
       <c r="AL52">
         <v>1</v>
       </c>
-      <c r="AM52" s="3">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="AN52">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AM52">
+        <v>1</v>
+      </c>
+      <c r="AN52" s="3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AO52">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>107</v>
       </c>
@@ -3277,12 +3403,15 @@
       <c r="AL53">
         <v>1</v>
       </c>
-      <c r="AM53" s="3">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AM53">
+        <v>1</v>
+      </c>
+      <c r="AN53" s="3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>109</v>
       </c>
@@ -3318,15 +3447,18 @@
       <c r="AK54">
         <v>1</v>
       </c>
-      <c r="AM54" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="AO54">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AL54">
+        <v>1</v>
+      </c>
+      <c r="AN54" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AP54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>111</v>
       </c>
@@ -3357,15 +3489,15 @@
         <f t="shared" ref="AF55:AF56" si="11">IF(OR(AG55=1,AH55=1),1,"")</f>
         <v/>
       </c>
-      <c r="AM55" s="3">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="AN55">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AN55" s="3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AO55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>63</v>
       </c>
@@ -3405,18 +3537,21 @@
       <c r="AL56">
         <v>1</v>
       </c>
-      <c r="AM56" s="3">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="AN56">
+      <c r="AM56">
+        <v>1</v>
+      </c>
+      <c r="AN56" s="3">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="AO56">
         <v>1</v>
       </c>
-    </row>
-    <row r="57" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AP56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>114</v>
       </c>
@@ -3449,18 +3584,18 @@
       <c r="AE57">
         <v>1</v>
       </c>
-      <c r="AM57" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="AO57">
-        <v>1</v>
-      </c>
-      <c r="AS57">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AN57" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AP57">
+        <v>1</v>
+      </c>
+      <c r="AT57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>116</v>
       </c>
@@ -3496,15 +3631,18 @@
       <c r="AL58">
         <v>1</v>
       </c>
-      <c r="AM58" s="3">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="AT58">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="59" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AM58">
+        <v>1</v>
+      </c>
+      <c r="AN58" s="3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AU58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>118</v>
       </c>
@@ -3535,18 +3673,18 @@
         <f>IF(OR(AG59=1,AH59=1),1,"")</f>
         <v/>
       </c>
-      <c r="AL59">
-        <v>1</v>
-      </c>
-      <c r="AM59" s="3">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="AN59">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AM59">
+        <v>1</v>
+      </c>
+      <c r="AN59" s="3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="AO59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>120</v>
       </c>
@@ -3579,12 +3717,12 @@
       <c r="AD60">
         <v>1</v>
       </c>
-      <c r="AM60" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="61" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AN60" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="61" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>122</v>
       </c>
@@ -3617,12 +3755,12 @@
       <c r="AH61">
         <v>1</v>
       </c>
-      <c r="AM61" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="62" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AN61" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="62" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>124</v>
       </c>
@@ -3652,12 +3790,12 @@
       <c r="AD62">
         <v>1</v>
       </c>
-      <c r="AM62" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="63" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AN62" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="63" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>126</v>
       </c>
@@ -3690,12 +3828,15 @@
       <c r="AK63">
         <v>1</v>
       </c>
-      <c r="AM63" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="64" spans="1:46" x14ac:dyDescent="0.25">
+      <c r="AL63">
+        <v>1</v>
+      </c>
+      <c r="AN63" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="64" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>128</v>
       </c>
@@ -3728,15 +3869,15 @@
       <c r="AE64">
         <v>1</v>
       </c>
-      <c r="AM64" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="AS64">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="AN64" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AT64">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>130</v>
       </c>
@@ -3773,12 +3914,12 @@
         <f t="shared" ref="AF65:AF66" si="12">IF(OR(AG65=1,AH65=1),1,"")</f>
         <v/>
       </c>
-      <c r="AM65" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-    </row>
-    <row r="66" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="AN65" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+    </row>
+    <row r="66" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>132</v>
       </c>
@@ -3812,15 +3953,15 @@
       <c r="AI66">
         <v>1</v>
       </c>
-      <c r="AM66" s="3" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="AR66">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="AN66" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="AS66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>134</v>
       </c>
@@ -3862,12 +4003,15 @@
       <c r="AL67">
         <v>1</v>
       </c>
-      <c r="AM67" s="3">
-        <f t="shared" ref="AM67:AM68" si="15">IF(OR(AN67=1,AL67=1),1,"")</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="AM67">
+        <v>1</v>
+      </c>
+      <c r="AN67" s="3">
+        <f t="shared" ref="AN67:AN68" si="15">IF(OR(AO67=1,AM67=1),1,"")</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>136</v>
       </c>
@@ -3907,12 +4051,15 @@
       <c r="AL68">
         <v>1</v>
       </c>
-      <c r="AM68" s="3">
+      <c r="AM68">
+        <v>1</v>
+      </c>
+      <c r="AN68" s="3">
         <f t="shared" si="15"/>
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>137</v>
       </c>
@@ -3926,7 +4073,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>138</v>
       </c>
@@ -3945,8 +4092,11 @@
       <c r="X70">
         <v>1</v>
       </c>
-    </row>
-    <row r="71" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="AL70">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>139</v>
       </c>
@@ -3968,8 +4118,11 @@
       <c r="AM71">
         <v>1</v>
       </c>
-    </row>
-    <row r="72" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="AN71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>140</v>
       </c>
@@ -3982,8 +4135,11 @@
       <c r="Y72">
         <v>1</v>
       </c>
-    </row>
-    <row r="73" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="AL72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>141</v>
       </c>
@@ -4009,7 +4165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>142</v>
       </c>
@@ -4034,22 +4190,25 @@
       <c r="AM74">
         <v>1</v>
       </c>
-    </row>
-    <row r="75" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="AN74">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>143</v>
       </c>
       <c r="C75" t="s">
         <v>175</v>
       </c>
-      <c r="AM75">
-        <v>1</v>
-      </c>
       <c r="AN75">
         <v>1</v>
       </c>
-    </row>
-    <row r="76" spans="1:44" x14ac:dyDescent="0.25">
+      <c r="AO75">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>144</v>
       </c>
@@ -4060,7 +4219,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>145</v>
       </c>
@@ -4068,7 +4227,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="78" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>146</v>
       </c>
@@ -4088,7 +4247,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>147</v>
       </c>
@@ -4108,7 +4267,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:44" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>148</v>
       </c>
@@ -4116,21 +4275,21 @@
         <v>175</v>
       </c>
     </row>
-    <row r="81" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>160</v>
       </c>
       <c r="C81" t="s">
         <v>175</v>
       </c>
-      <c r="AO81">
-        <v>1</v>
-      </c>
-      <c r="AS81">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="82" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AP81">
+        <v>1</v>
+      </c>
+      <c r="AT81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>161</v>
       </c>
@@ -4148,7 +4307,11 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AT82"/>
+  <autoFilter ref="A1:AU82">
+    <filterColumn colId="37">
+      <filters blank="1"/>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Change: allow WDPR (timber) on flat wagons
</commit_message>
<xml_diff>
--- a/docs/cargo_classes.xlsx
+++ b/docs/cargo_classes.xlsx
@@ -926,14 +926,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:AU82"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="E54" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2:B66"/>
+      <selection pane="bottomRight" activeCell="AF66" sqref="AF66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1180,7 +1179,7 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1309,7 +1308,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -1363,7 +1362,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -1526,7 +1525,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -1568,7 +1567,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -1613,7 +1612,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>29</v>
       </c>
@@ -1654,7 +1653,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -1711,7 +1710,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -1753,7 +1752,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:46" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -1797,7 +1796,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:46" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>37</v>
       </c>
@@ -1844,7 +1843,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:46" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>39</v>
       </c>
@@ -1920,7 +1919,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:46" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>43</v>
       </c>
@@ -1965,7 +1964,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:46" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>45</v>
       </c>
@@ -2007,7 +2006,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:46" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>47</v>
       </c>
@@ -2054,7 +2053,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:46" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>49</v>
       </c>
@@ -2093,7 +2092,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:46" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>51</v>
       </c>
@@ -2132,7 +2131,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:46" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>53</v>
       </c>
@@ -2171,7 +2170,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:46" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>55</v>
       </c>
@@ -2210,7 +2209,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:46" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>57</v>
       </c>
@@ -2252,7 +2251,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:46" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>59</v>
       </c>
@@ -2291,7 +2290,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:46" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>61</v>
       </c>
@@ -2330,7 +2329,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:46" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>63</v>
       </c>
@@ -2378,7 +2377,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:46" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:46" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>65</v>
       </c>
@@ -2458,7 +2457,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>69</v>
       </c>
@@ -2515,7 +2514,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>71</v>
       </c>
@@ -2572,7 +2571,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>73</v>
       </c>
@@ -2613,7 +2612,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>75</v>
       </c>
@@ -2655,7 +2654,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>77</v>
       </c>
@@ -2738,7 +2737,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>81</v>
       </c>
@@ -2791,7 +2790,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>83</v>
       </c>
@@ -2833,7 +2832,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>85</v>
       </c>
@@ -2881,7 +2880,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>87</v>
       </c>
@@ -2932,7 +2931,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>89</v>
       </c>
@@ -2985,7 +2984,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>91</v>
       </c>
@@ -3032,7 +3031,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>93</v>
       </c>
@@ -3086,7 +3085,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>95</v>
       </c>
@@ -3140,7 +3139,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>97</v>
       </c>
@@ -3191,7 +3190,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>99</v>
       </c>
@@ -3312,7 +3311,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>105</v>
       </c>
@@ -3366,7 +3365,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>107</v>
       </c>
@@ -3411,7 +3410,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>109</v>
       </c>
@@ -3497,7 +3496,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>63</v>
       </c>
@@ -3595,7 +3594,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>116</v>
       </c>
@@ -3795,7 +3794,7 @@
         <v/>
       </c>
     </row>
-    <row r="63" spans="1:47" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>126</v>
       </c>
@@ -3961,7 +3960,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>134</v>
       </c>
@@ -3994,6 +3993,9 @@
       <c r="AD67">
         <v>1</v>
       </c>
+      <c r="AF67">
+        <v>1</v>
+      </c>
       <c r="AG67">
         <v>1</v>
       </c>
@@ -4011,7 +4013,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>136</v>
       </c>
@@ -4073,7 +4075,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>138</v>
       </c>
@@ -4096,7 +4098,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>139</v>
       </c>
@@ -4122,7 +4124,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>140</v>
       </c>
@@ -4165,7 +4167,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>142</v>
       </c>
@@ -4307,11 +4309,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AU82">
-    <filterColumn colId="37">
-      <filters blank="1"/>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:AU82"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>